<commit_message>
Errores raros en el commit
</commit_message>
<xml_diff>
--- a/SpaOnline/ModeloDominio/Facturacion - Muestreo Datos.xlsx
+++ b/SpaOnline/ModeloDominio/Facturacion - Muestreo Datos.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grchia-my.sharepoint.com/personal/jhonatan_gomez_wiga_io/Documents/Escritorio/UCO/DOO/SpaOnline/ModeloDominio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{7AD8AF4F-42CC-425B-8D43-A34E7CA0C0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5958AEF-4A2B-4F85-BF23-24E3301AEF32}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{7AD8AF4F-42CC-425B-8D43-A34E7CA0C0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66787ECE-53EA-4C8C-A118-431E8460F11E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="774" activeTab="4" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo de Dominio Anemico" sheetId="1" r:id="rId1"/>
     <sheet name="Objetos de dominio" sheetId="2" r:id="rId2"/>
-    <sheet name="Pagos" sheetId="5" r:id="rId3"/>
-    <sheet name="Factura" sheetId="6" r:id="rId4"/>
-    <sheet name="Reserva" sheetId="7" r:id="rId5"/>
+    <sheet name="ProductoInventario" sheetId="8" r:id="rId3"/>
+    <sheet name="Pagos" sheetId="5" r:id="rId4"/>
+    <sheet name="Factura" sheetId="6" r:id="rId5"/>
+    <sheet name="Reserva" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
   <si>
     <t xml:space="preserve">Nombre </t>
   </si>
@@ -143,9 +144,6 @@
     <t>Cliente</t>
   </si>
   <si>
-    <t>Servicio</t>
-  </si>
-  <si>
     <t>ValorTotal</t>
   </si>
   <si>
@@ -180,6 +178,51 @@
   </si>
   <si>
     <t>12:30pm - 05/05/2024</t>
+  </si>
+  <si>
+    <t>ProductoInventario</t>
+  </si>
+  <si>
+    <t>Objeto de dominio que contiene la informacion de los  producto inventario para discriminar de que inventario se esta sacando un producto a la hora de facturar</t>
+  </si>
+  <si>
+    <t>Inventarios</t>
+  </si>
+  <si>
+    <t>Producto</t>
+  </si>
+  <si>
+    <t>Cantidad Productos</t>
+  </si>
+  <si>
+    <t>PrecioCompraU</t>
+  </si>
+  <si>
+    <t>FechaCompra</t>
+  </si>
+  <si>
+    <t>Combinacion Unica</t>
+  </si>
+  <si>
+    <t>Crema de Día anti-edad - L'Oréal</t>
+  </si>
+  <si>
+    <t>Demalogica Daily Microfoliant - Dernalogica</t>
+  </si>
+  <si>
+    <t>Daily Moisture lotion - Lubriderm</t>
+  </si>
+  <si>
+    <t>Notificado</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Pagado</t>
+  </si>
+  <si>
+    <t>False</t>
   </si>
 </sst>
 </file>
@@ -190,7 +233,7 @@
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +250,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u val="singleAccounting"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -262,7 +321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -280,6 +339,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -308,17 +382,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>601010</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>124374</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>363188</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>67466</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
+        <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7147DC95-0BE3-9DA1-6F37-7E962E1306AA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCBD71D5-48AC-4569-AEED-E812226C5E53}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -335,7 +409,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6697010" cy="3934374"/>
+          <a:ext cx="7983188" cy="6353966"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -683,7 +757,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,15 +772,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D92343-C7F8-498A-9249-704487594109}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="68" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -731,7 +805,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>4</v>
@@ -756,7 +830,7 @@
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -765,7 +839,21 @@
         <v>24</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -775,6 +863,108 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB81781-599A-46BA-9C29-6B7C45668086}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="6" max="6" width="43.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="1">
+        <v>10</v>
+      </c>
+      <c r="D2" s="12">
+        <v>12000</v>
+      </c>
+      <c r="E2" s="13">
+        <v>45369</v>
+      </c>
+      <c r="F2" s="14" t="str">
+        <f>B2</f>
+        <v>Crema de Día anti-edad - L'Oréal</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="1">
+        <v>50</v>
+      </c>
+      <c r="D3" s="12">
+        <v>20000</v>
+      </c>
+      <c r="E3" s="13">
+        <v>45346</v>
+      </c>
+      <c r="F3" s="14" t="str">
+        <f>B3</f>
+        <v>Demalogica Daily Microfoliant - Dernalogica</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="1">
+        <v>100</v>
+      </c>
+      <c r="D4" s="12">
+        <v>14500</v>
+      </c>
+      <c r="E4" s="13">
+        <v>45262</v>
+      </c>
+      <c r="F4" s="14" t="str">
+        <f>B4</f>
+        <v>Daily Moisture lotion - Lubriderm</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952BDDC5-1485-4BC4-A31B-18839936F54D}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -841,23 +1031,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AC5A6C-A671-4129-B9B4-327F158A64E8}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -865,80 +1058,122 @@
         <v>26</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="9">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2" t="str">
+        <f>ProductoInventario!F2 &amp;"  "&amp;ProductoInventario!F3</f>
+        <v>Crema de Día anti-edad - L'Oréal  Demalogica Daily Microfoliant - Dernalogica</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="9">
         <v>220000</v>
       </c>
-      <c r="E2" s="5" t="str">
+      <c r="H2" s="5" t="str">
         <f>B2</f>
         <v>Martina Corrales-1234567890</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="2"/>
+      <c r="E3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="15">
         <v>120000</v>
       </c>
-      <c r="E3" s="5" t="str">
-        <f t="shared" ref="E3:E4" si="0">B3</f>
+      <c r="H3" s="5" t="str">
+        <f t="shared" ref="H3:H4" si="0">B3</f>
         <v>Ramiro Ramirez-987654321</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="2" t="str">
+        <f>ProductoInventario!F4</f>
+        <v>Daily Moisture lotion - Lubriderm</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="9">
         <v>100000</v>
       </c>
-      <c r="E4" s="5" t="str">
+      <c r="H4" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Lucrecia Gomez-39789321</v>
       </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="16"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A94161E0-3BD5-4F6A-BC3F-F11C41E66D7B}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,7 +1194,7 @@
         <v>26</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>22</v>
@@ -976,10 +1211,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -997,10 +1232,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>18</v>
@@ -1018,10 +1253,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Corrección muestreo de datos
</commit_message>
<xml_diff>
--- a/SpaOnline/ModeloDominio/Facturacion - Muestreo Datos.xlsx
+++ b/SpaOnline/ModeloDominio/Facturacion - Muestreo Datos.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis ospina\OneDrive\Documentos\GitHub\DOO\SpaOnline\ModeloDominio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DOO\DOO\SpaOnline\ModeloDominio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE1ED92-6E25-4C61-BDB8-8A95E1FFF680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E896BD3-D773-495A-9BF0-531994BA39C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="774" activeTab="4" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo de Dominio Anemico" sheetId="1" r:id="rId1"/>
     <sheet name="Objetos de dominio" sheetId="2" r:id="rId2"/>
-    <sheet name="ProductoInventario" sheetId="8" r:id="rId3"/>
+    <sheet name="Notificacion" sheetId="9" r:id="rId3"/>
     <sheet name="Pagos" sheetId="5" r:id="rId4"/>
     <sheet name="Factura" sheetId="6" r:id="rId5"/>
     <sheet name="Reserva" sheetId="7" r:id="rId6"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
   <si>
     <t xml:space="preserve">Nombre </t>
   </si>
@@ -113,15 +113,6 @@
     <t>Sucursal</t>
   </si>
   <si>
-    <t>Rionegro-Antioquia-Colombia-CL 10 43 A 29</t>
-  </si>
-  <si>
-    <t>Marinilla-Antioquia-Colombia-CL 63 9 36</t>
-  </si>
-  <si>
-    <t>Medellin-Antioquia-Colombia-CR 2 5 39</t>
-  </si>
-  <si>
     <t>Reserva</t>
   </si>
   <si>
@@ -137,18 +128,6 @@
     <t>Cliente</t>
   </si>
   <si>
-    <t>ValorTotal</t>
-  </si>
-  <si>
-    <t>Martina Corrales-1234567890</t>
-  </si>
-  <si>
-    <t>Ramiro Ramirez-987654321</t>
-  </si>
-  <si>
-    <t>Lucrecia Gomez-39789321</t>
-  </si>
-  <si>
     <t>Pagos</t>
   </si>
   <si>
@@ -161,27 +140,6 @@
     <t>Agenda</t>
   </si>
   <si>
-    <t>ProductoInventario</t>
-  </si>
-  <si>
-    <t>Objeto de dominio que contiene la informacion de los  producto inventario para discriminar de que inventario se esta sacando un producto a la hora de facturar</t>
-  </si>
-  <si>
-    <t>Inventarios</t>
-  </si>
-  <si>
-    <t>Producto</t>
-  </si>
-  <si>
-    <t>Cantidad Productos</t>
-  </si>
-  <si>
-    <t>PrecioCompraU</t>
-  </si>
-  <si>
-    <t>FechaCompra</t>
-  </si>
-  <si>
     <t>Notificado</t>
   </si>
   <si>
@@ -203,34 +161,61 @@
     <t>Lucrecia Gomez</t>
   </si>
   <si>
-    <t>Inventario</t>
-  </si>
-  <si>
-    <t>PrecioVenta</t>
-  </si>
-  <si>
     <t>Detalle Reserva</t>
   </si>
   <si>
     <t>Detalle de Reserva</t>
   </si>
   <si>
-    <t>ValorReserva</t>
-  </si>
-  <si>
-    <t>Detalle Factura</t>
-  </si>
-  <si>
-    <t>Pais}</t>
-  </si>
-  <si>
-    <t>Colimbia</t>
-  </si>
-  <si>
-    <t>Departanenbos</t>
-  </si>
-  <si>
-    <t>Antioquia - Cyubducinarca - guarhura ----</t>
+    <t>Consentimiento</t>
+  </si>
+  <si>
+    <t>ReservaNotificada</t>
+  </si>
+  <si>
+    <t>Tarifa</t>
+  </si>
+  <si>
+    <t>ValorAPagar</t>
+  </si>
+  <si>
+    <t>TipoNotificacion</t>
+  </si>
+  <si>
+    <t>NotificadoA</t>
+  </si>
+  <si>
+    <t>Mesaje</t>
+  </si>
+  <si>
+    <t>EsNotificado</t>
+  </si>
+  <si>
+    <t>La reserva ha sido realizada exitosamente</t>
+  </si>
+  <si>
+    <t>Queremos informarte que por el mes de madres hay descuento en limpieza facial</t>
+  </si>
+  <si>
+    <t>Le adjuntamos su factura emitida</t>
+  </si>
+  <si>
+    <t>Notificación</t>
+  </si>
+  <si>
+    <t>Objeto de dominio que contiene la informacion de las notificaciones que emite el Spa</t>
+  </si>
+  <si>
+    <t>Factura 1</t>
+  </si>
+  <si>
+    <t>Factura 2</t>
+  </si>
+  <si>
+    <t>Factura 3</t>
+  </si>
+  <si>
+    <t>Nombre Factura</t>
   </si>
 </sst>
 </file>
@@ -240,9 +225,9 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-[$$-240A]\ * #,##0.00_-;\-[$$-240A]\ * #,##0.00_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-[$$-240A]\ * #,##0_-;\-[$$-240A]\ * #,##0_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,6 +266,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -302,7 +293,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -325,13 +316,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -347,26 +349,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -398,17 +396,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>363188</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>67466</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>181957</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76663</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCBD71D5-48AC-4569-AEED-E812226C5E53}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{522A60EF-0950-6483-9A03-C485470A6949}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -425,7 +423,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7983188" cy="6353966"/>
+          <a:ext cx="7039957" cy="3315163"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -446,54 +444,7 @@
     <sheetNames>
       <sheetName val="Modelo de Dominio Anemico"/>
       <sheetName val="Objetos de dominio"/>
-      <sheetName val="ProductoInventario"/>
-      <sheetName val="Inventario"/>
-      <sheetName val="Sucursal"/>
-      <sheetName val="Producto"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3">
-        <row r="2">
-          <cell r="B2" t="str">
-            <v>Inventario A</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5">
-        <row r="2">
-          <cell r="B2" t="str">
-            <v>Crema de Día Anti-edad</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3" t="str">
-            <v>Dermalogica Daily Microfoliant</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4" t="str">
-            <v>Daily Moisture Lotion</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Modelo de Dominio Anemico"/>
-      <sheetName val="Objetos de dominio"/>
+      <sheetName val="Notificaciones"/>
       <sheetName val="Cliente"/>
       <sheetName val="Servicio"/>
       <sheetName val="Reserva"/>
@@ -504,13 +455,20 @@
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3">
+      <sheetData sheetId="2">
+        <row r="2">
+          <cell r="E2" t="str">
+            <v>True</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4">
         <row r="2">
           <cell r="B2" t="str">
             <v>Pedicura Spa</v>
           </cell>
-          <cell r="E2">
+          <cell r="C2">
             <v>100000</v>
           </cell>
         </row>
@@ -518,7 +476,7 @@
           <cell r="B3" t="str">
             <v>Tratamiento Facial Antiedad</v>
           </cell>
-          <cell r="E3">
+          <cell r="C3">
             <v>120000</v>
           </cell>
         </row>
@@ -526,21 +484,53 @@
           <cell r="B4" t="str">
             <v>Masaje Relajante</v>
           </cell>
-          <cell r="E4">
+          <cell r="C4">
             <v>100000</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
+      <sheetData sheetId="6">
+        <row r="2">
+          <cell r="D2" t="str">
+            <v>True</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="D3" t="str">
+            <v>False</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="D4" t="str">
+            <v>True</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="7">
+        <row r="2">
+          <cell r="C2" t="str">
+            <v>Sucursal Rionegro</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="C3" t="str">
+            <v>Sucursal Marinilla</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="C4" t="str">
+            <v>Sucursal El Poblado</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="8"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -578,6 +568,65 @@
         <row r="4">
           <cell r="E4" t="str">
             <v>2:00pm-3:00pm-05/05/2024</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Modelo de Dominio Anemico"/>
+      <sheetName val="Objetos de dominio"/>
+      <sheetName val="Notificación"/>
+      <sheetName val="Cliente"/>
+      <sheetName val="TipoNotificación"/>
+      <sheetName val="ListaNotificacion"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3">
+        <row r="2">
+          <cell r="G2" t="str">
+            <v>martina.corrales@gmail.com</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="G4" t="str">
+            <v>lucrecia.gomez@hotmail.com</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4">
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>Reserva</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>Evento</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>Factura</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5">
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>General</v>
           </cell>
         </row>
       </sheetData>
@@ -919,34 +968,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA198BEE-AB41-4447-8B76-5672FB9C01F4}">
-  <dimension ref="N13:O14"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="11.42578125" style="7"/>
   </cols>
-  <sheetData>
-    <row r="13" spans="14:15" x14ac:dyDescent="0.25">
-      <c r="N13" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="O13" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="14:15" x14ac:dyDescent="0.25">
-      <c r="N14" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="O14" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -957,7 +989,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,7 +997,7 @@
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="68" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -983,11 +1015,11 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>4</v>
@@ -997,177 +1029,152 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>29</v>
+      <c r="A4" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>31</v>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>33</v>
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" location="Factura!A1" display="Factura" xr:uid="{1C2141E3-8011-42A8-9026-15E7D61C7C1B}"/>
+    <hyperlink ref="A3" location="Reserva!A1" display="Reserva" xr:uid="{2EB85D99-B13D-44B2-9AE0-8E87AD0FE770}"/>
+    <hyperlink ref="A4" location="Pagos!A1" display="Pago" xr:uid="{3F1122AC-9E92-44C7-8225-1EB80C1BA9C6}"/>
+    <hyperlink ref="A5" location="Notificacion!A1" display="Notificación" xr:uid="{D4C48AC5-11B5-4BBE-BAA4-E77E1FF79F95}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB81781-599A-46BA-9C29-6B7C45668086}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD5A6E6-0C94-40D1-927D-4AB84E837D70}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="str">
-        <f>[1]Inventario!B2</f>
-        <v>Inventario A</v>
+      <c r="B2" s="10" t="str">
+        <f>+[3]TipoNotificación!B2</f>
+        <v>Reserva</v>
       </c>
       <c r="C2" s="1" t="str">
-        <f>[1]Producto!B2</f>
-        <v>Crema de Día Anti-edad</v>
-      </c>
-      <c r="D2" s="1">
-        <v>10</v>
-      </c>
-      <c r="E2" s="15">
-        <f>(F2*15%)+F2</f>
-        <v>13800</v>
-      </c>
-      <c r="F2" s="9">
-        <v>12000</v>
-      </c>
-      <c r="G2" s="10">
-        <v>45369</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+        <f>[3]Cliente!G2</f>
+        <v>martina.corrales@gmail.com</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="str">
-        <f>[1]Inventario!B2</f>
-        <v>Inventario A</v>
+      <c r="B3" s="10" t="str">
+        <f>+[3]TipoNotificación!B3</f>
+        <v>Evento</v>
       </c>
       <c r="C3" s="1" t="str">
-        <f>[1]Producto!B3</f>
-        <v>Dermalogica Daily Microfoliant</v>
-      </c>
-      <c r="D3" s="1">
-        <v>50</v>
-      </c>
-      <c r="E3" s="15">
-        <f t="shared" ref="E3:E4" si="0">(F3*15%)+F3</f>
-        <v>23000</v>
-      </c>
-      <c r="F3" s="9">
-        <v>20000</v>
-      </c>
-      <c r="G3" s="10">
-        <v>45346</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+        <f>+[3]ListaNotificacion!B2</f>
+        <v>General</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="str">
-        <f>[1]Inventario!B2</f>
-        <v>Inventario A</v>
+      <c r="B4" s="10" t="str">
+        <f>+[3]TipoNotificación!B4</f>
+        <v>Factura</v>
       </c>
       <c r="C4" s="1" t="str">
-        <f>[1]Producto!B4</f>
-        <v>Daily Moisture Lotion</v>
-      </c>
-      <c r="D4" s="1">
-        <v>100</v>
-      </c>
-      <c r="E4" s="15">
-        <f t="shared" si="0"/>
-        <v>16675</v>
-      </c>
-      <c r="F4" s="9">
-        <v>14500</v>
-      </c>
-      <c r="G4" s="10">
-        <v>45262</v>
+        <f>[3]Cliente!G4</f>
+        <v>lucrecia.gomez@hotmail.com</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" location="Inventario!B2" display="Inventario!B2" xr:uid="{FE4766DD-85C1-4403-A449-D9A21D82D3F6}"/>
-    <hyperlink ref="B3" location="Inventario!B2" display="Inventario!B2" xr:uid="{1C3F4C2C-53CB-4B0E-98FC-0F2C4A745007}"/>
-    <hyperlink ref="B4" location="Inventario!A1" display="Inventario!A1" xr:uid="{D25698F5-7C45-4E1C-87D7-FABA581FEEF4}"/>
+    <hyperlink ref="B2" location="TipoNotificación!A1" display="TipoNotificación!A1" xr:uid="{EFD773F4-A951-433E-8CB5-EF69F2FE40CD}"/>
+    <hyperlink ref="B3" location="TipoNotificación!A1" display="TipoNotificación!A1" xr:uid="{05A01EE5-9B74-41D1-8416-B2A0000C6DDC}"/>
+    <hyperlink ref="B4" location="TipoNotificación!A1" display="TipoNotificación!A1" xr:uid="{69F1AB61-DCBA-417E-B95E-F834ADE3FCEC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1178,7 +1185,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,278 +1233,308 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AC5A6C-A671-4129-B9B4-327F158A64E8}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="55.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="13" t="str">
-        <f>Reserva!C2</f>
-        <v>Pedicura Spa</v>
-      </c>
-      <c r="D2" s="13" t="str">
-        <f>ProductoInventario!C2 &amp; " + "&amp;ProductoInventario!C3</f>
-        <v>Crema de Día Anti-edad + Dermalogica Daily Microfoliant</v>
-      </c>
-      <c r="E2" s="16" t="str">
-        <f>C2&amp;" + " &amp;D2</f>
-        <v>Pedicura Spa + Crema de Día Anti-edad + Dermalogica Daily Microfoliant</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="18" t="str">
-        <f>Reserva!D2 &amp;" + "&amp;ProductoInventario!E2 &amp;" + "&amp;ProductoInventario!E3</f>
-        <v>100000 + 13800 + 23000</v>
-      </c>
-      <c r="I2" s="5" t="str">
-        <f>B2</f>
-        <v>Martina Corrales-1234567890</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="13" t="str">
-        <f>Reserva!C3</f>
-        <v>Tratamiento Facial Antiedad</v>
-      </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13" t="str">
-        <f>C3</f>
-        <v>Tratamiento Facial Antiedad</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="17">
-        <f>Reserva!D3</f>
-        <v>120000</v>
-      </c>
-      <c r="I3" s="5" t="str">
-        <f t="shared" ref="I3:I4" si="0">B3</f>
-        <v>Ramiro Ramirez-987654321</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="13" t="str">
-        <f>Reserva!C4</f>
-        <v>Masaje Relajante</v>
-      </c>
-      <c r="D4" s="13" t="str">
-        <f>ProductoInventario!C4</f>
-        <v>Daily Moisture Lotion</v>
-      </c>
-      <c r="E4" s="13" t="str">
-        <f>C4&amp;" + " &amp; D4</f>
-        <v>Masaje Relajante + Daily Moisture Lotion</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="17" t="str">
-        <f>Reserva!D4&amp;" + " &amp;ProductoInventario!E4</f>
-        <v>100000 + 16675</v>
-      </c>
-      <c r="I4" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Lucrecia Gomez-39789321</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G9" s="11"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" location="Reserva!A1" display="Reserva!A1" xr:uid="{6947F9A6-4041-47C7-AC78-B2E530E84F7E}"/>
-    <hyperlink ref="C3:C4" location="Reserva!A1" display="Reserva!A1" xr:uid="{B8B87086-BD94-4A82-ACEC-73402F9801B0}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A94161E0-3BD5-4F6A-BC3F-F11C41E66D7B}">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="13" t="str">
-        <f>[2]Servicio!B2</f>
+      <c r="B2" s="10" t="str">
+        <f>+Reserva!B2</f>
+        <v>Martina Corrales</v>
+      </c>
+      <c r="C2" s="10" t="str">
+        <f>Reserva!C2</f>
         <v>Pedicura Spa</v>
       </c>
-      <c r="D2" s="12">
-        <f>[2]Servicio!E2</f>
+      <c r="D2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="10" t="str">
+        <f>+Notificacion!E2</f>
+        <v>True</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="16">
+        <f>+Reserva!F2</f>
         <v>100000</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="13" t="str">
-        <f>[3]Agenda!E2</f>
-        <v>3:00pm-4:00pm-16/03/2024</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" s="5" t="str">
+        <f>+D2&amp;"-"&amp;C2&amp;"-"&amp;G2</f>
+        <v>Factura 1-Pedicura Spa-100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="13" t="str">
-        <f>[2]Servicio!B3</f>
+      <c r="B3" s="10" t="str">
+        <f>+Reserva!B3</f>
+        <v>Ramiro Ramirez</v>
+      </c>
+      <c r="C3" s="10" t="str">
+        <f>Reserva!C3</f>
         <v>Tratamiento Facial Antiedad</v>
       </c>
-      <c r="D3" s="12">
-        <f>[2]Servicio!E3</f>
+      <c r="D3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="10" t="str">
+        <f>+Notificacion!E3</f>
+        <v>True</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="16">
+        <f>+Reserva!F3</f>
         <v>120000</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="13" t="str">
-        <f>[3]Agenda!E3</f>
-        <v>11:00am-12:00pm-28/04/2024</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" s="5" t="str">
+        <f t="shared" ref="H3:H4" si="0">+D3&amp;"-"&amp;C3&amp;"-"&amp;G3</f>
+        <v>Factura 2-Tratamiento Facial Antiedad-120000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="13" t="str">
-        <f>[2]Servicio!B4</f>
+      <c r="B4" s="10" t="str">
+        <f>+Reserva!B4</f>
+        <v>Lucrecia Gomez</v>
+      </c>
+      <c r="C4" s="10" t="str">
+        <f>Reserva!C4</f>
         <v>Masaje Relajante</v>
       </c>
-      <c r="D4" s="12">
-        <f>[2]Servicio!E4</f>
+      <c r="D4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="10" t="str">
+        <f>+Notificacion!E4</f>
+        <v>False</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="16">
+        <f>+Reserva!F4</f>
         <v>100000</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="13" t="str">
-        <f>[3]Agenda!E4</f>
-        <v>2:00pm-3:00pm-05/05/2024</v>
-      </c>
+      <c r="H4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Factura 3-Masaje Relajante-100000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="9"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" location="ReservaServicio!B2" display="Pedicura Spa-Masaje Relajante" xr:uid="{C1819DAD-8843-4AD5-8482-7E38683B29D0}"/>
-    <hyperlink ref="C3:C4" location="ReservaServicio!B2" display="Pedicura Spa-Masaje Relajante" xr:uid="{E3265642-EF4B-447C-9E1D-DF1B2ED88CA8}"/>
-    <hyperlink ref="F2" location="Agenda!A1" display="Agenda!A1" xr:uid="{CEFAEFDC-CD77-40F7-B3EA-8854981749F6}"/>
-    <hyperlink ref="F3" location="Agenda!A1" display="Agenda!A1" xr:uid="{49237E06-2916-4AAD-B5BE-C628FA344E0C}"/>
-    <hyperlink ref="F4" location="Agenda!A1" display="Agenda!A1" xr:uid="{1BBF8CCB-FAEC-4AFD-8A6A-BB758513E0D9}"/>
+    <hyperlink ref="C2" location="Reserva!A1" display="Reserva!A1" xr:uid="{6947F9A6-4041-47C7-AC78-B2E530E84F7E}"/>
+    <hyperlink ref="C3:C4" location="Reserva!A1" display="Reserva!A1" xr:uid="{B8B87086-BD94-4A82-ACEC-73402F9801B0}"/>
+    <hyperlink ref="B2" location="Reserva!B2" display="Reserva!B2" xr:uid="{06E39748-4FA0-477D-B883-885C35213D4B}"/>
+    <hyperlink ref="B3" location="Reserva!B3" display="Reserva!B3" xr:uid="{D908D230-F46A-4FA9-A20B-1D65478D8D71}"/>
+    <hyperlink ref="B4" location="Reserva!B4" display="Reserva!B4" xr:uid="{410D0A96-14D2-45F1-919A-70AD0ED3C629}"/>
+    <hyperlink ref="E2" location="Notificacion!B2" display="Notificacion!B2" xr:uid="{7A48BB80-9C87-4B1F-ACE0-4F744CF2AA89}"/>
+    <hyperlink ref="E3" location="Factura!B3" display="Factura!B3" xr:uid="{8179C6C9-E0EB-4566-9571-C35246FED464}"/>
+    <hyperlink ref="E4" location="Factura!B3" display="Factura!B3" xr:uid="{40334A43-D75F-405D-931F-DDFA4B141F40}"/>
+    <hyperlink ref="G2" location="Reserva!A1" display="Reserva!A1" xr:uid="{F8410D16-6435-4D47-B8B4-A083346AD047}"/>
+    <hyperlink ref="G3" location="Factura!B3" display="Factura!B3" xr:uid="{DED59F6F-B19B-4087-886B-BD4E5BD0DB03}"/>
+    <hyperlink ref="G4" location="Factura!B4" display="Factura!B4" xr:uid="{391633E6-292C-4B92-810D-19E4E77F0D42}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A94161E0-3BD5-4F6A-BC3F-F11C41E66D7B}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="15" t="str">
+        <f>[1]Servicio!B2</f>
+        <v>Pedicura Spa</v>
+      </c>
+      <c r="D2" s="15" t="str">
+        <f>+[1]Sucursal!C2</f>
+        <v>Sucursal Rionegro</v>
+      </c>
+      <c r="E2" s="15" t="str">
+        <f>[2]Agenda!E2</f>
+        <v>3:00pm-4:00pm-16/03/2024</v>
+      </c>
+      <c r="F2" s="14">
+        <f>+[1]Servicio!C2</f>
+        <v>100000</v>
+      </c>
+      <c r="G2" s="13" t="str">
+        <f>+[1]Consentimiento!D2</f>
+        <v>True</v>
+      </c>
+      <c r="H2" s="13" t="str">
+        <f>+[1]Notificaciones!E2</f>
+        <v>True</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="15" t="str">
+        <f>[1]Servicio!B3</f>
+        <v>Tratamiento Facial Antiedad</v>
+      </c>
+      <c r="D3" s="15" t="str">
+        <f>+[1]Sucursal!C3</f>
+        <v>Sucursal Marinilla</v>
+      </c>
+      <c r="E3" s="15" t="str">
+        <f>[2]Agenda!E3</f>
+        <v>11:00am-12:00pm-28/04/2024</v>
+      </c>
+      <c r="F3" s="14">
+        <f>+[1]Servicio!C3</f>
+        <v>120000</v>
+      </c>
+      <c r="G3" s="13" t="str">
+        <f>+[1]Consentimiento!D3</f>
+        <v>False</v>
+      </c>
+      <c r="H3" s="13" t="str">
+        <f>+[1]Notificaciones!E2</f>
+        <v>True</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="15" t="str">
+        <f>[1]Servicio!B4</f>
+        <v>Masaje Relajante</v>
+      </c>
+      <c r="D4" s="15" t="str">
+        <f>+[1]Sucursal!C4</f>
+        <v>Sucursal El Poblado</v>
+      </c>
+      <c r="E4" s="15" t="str">
+        <f>[2]Agenda!E4</f>
+        <v>2:00pm-3:00pm-05/05/2024</v>
+      </c>
+      <c r="F4" s="14">
+        <f>+[1]Servicio!C4</f>
+        <v>100000</v>
+      </c>
+      <c r="G4" s="13" t="str">
+        <f>+[1]Consentimiento!D4</f>
+        <v>True</v>
+      </c>
+      <c r="H4" s="13" t="str">
+        <f>+[1]Notificaciones!E2</f>
+        <v>True</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>